<commit_message>
[STABLE] IPv4 and IPv6 Routing Working (incomplete)
</commit_message>
<xml_diff>
--- a/Phase 1/AR-Presentation/AR-Phase1.xlsx
+++ b/Phase 1/AR-Presentation/AR-Phase1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Universidade de Aveiro\Paulo Vasconcelos - Projeto Final\Phase 1\AR-Presentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B47BBB-3938-49F3-A610-0D49F3EDF558}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10466BCD-23A4-40D8-A5E5-2B94BEF77EDB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0A47DF32-7327-452B-A5C9-3BA160086B8C}"/>
   </bookViews>
@@ -1159,6 +1159,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1171,89 +1246,14 @@
     <xf numFmtId="1" fontId="6" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="6" fillId="6" borderId="2" xfId="5" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1801,46 +1801,46 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:27" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="73"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="72"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="71" t="s">
+      <c r="G3" s="53"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="70" t="s">
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="O3" s="70"/>
-      <c r="P3" s="70"/>
-      <c r="Q3" s="70"/>
-      <c r="R3" s="70"/>
-      <c r="S3" s="58" t="s">
+      <c r="O3" s="51"/>
+      <c r="P3" s="51"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="51"/>
+      <c r="S3" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58" t="s">
+      <c r="T3" s="55"/>
+      <c r="U3" s="55"/>
+      <c r="V3" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58" t="s">
+      <c r="W3" s="55"/>
+      <c r="X3" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="Y3" s="58"/>
+      <c r="Y3" s="55"/>
       <c r="Z3" s="22"/>
       <c r="AA3" s="22"/>
     </row>
@@ -1921,13 +1921,13 @@
       <c r="AA4" s="22"/>
     </row>
     <row r="5" spans="2:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="47">
+      <c r="C5" s="45">
         <v>1</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="45" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="2">
@@ -1939,7 +1939,7 @@
       <c r="G5" s="2">
         <v>2</v>
       </c>
-      <c r="H5" s="74" t="s">
+      <c r="H5" s="49" t="s">
         <v>46</v>
       </c>
       <c r="I5" s="3">
@@ -1967,43 +1967,43 @@
         <f t="shared" ref="O5:O29" si="3">IF(F5="VoIP", N5, 0)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="47">
+      <c r="P5" s="45">
         <f>SUM(N5:N6)</f>
         <v>60</v>
       </c>
-      <c r="Q5" s="47">
+      <c r="Q5" s="45">
         <f>SUM(O5:O6)</f>
         <v>20</v>
       </c>
-      <c r="R5" s="61">
+      <c r="R5" s="43">
         <f>SUM(M5:M6)</f>
         <v>32.625</v>
       </c>
-      <c r="S5" s="47">
+      <c r="S5" s="45">
         <f>SUM(P5:P15)</f>
         <v>522</v>
       </c>
-      <c r="T5" s="60">
+      <c r="T5" s="46">
         <f>S5/$C$44</f>
         <v>10.875</v>
       </c>
-      <c r="U5" s="47">
+      <c r="U5" s="45">
         <f>SUM(M5:M15)</f>
         <v>712.78750000000002</v>
       </c>
-      <c r="V5" s="47">
+      <c r="V5" s="45">
         <f>U5+U16*C34+U22</f>
         <v>3324.8874999999998</v>
       </c>
-      <c r="W5" s="60">
+      <c r="W5" s="46">
         <f>T5+T16*C34+T22</f>
         <v>39.875</v>
       </c>
-      <c r="X5" s="43">
+      <c r="X5" s="68">
         <f>V5*AA5+T30</f>
         <v>13312.05</v>
       </c>
-      <c r="Y5" s="45">
+      <c r="Y5" s="70">
         <f>W5*AA5+T30</f>
         <v>172</v>
       </c>
@@ -2015,9 +2015,9 @@
       </c>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B6" s="66"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
       <c r="E6" s="2">
         <v>20</v>
       </c>
@@ -2027,7 +2027,7 @@
       <c r="G6" s="2">
         <v>1</v>
       </c>
-      <c r="H6" s="74"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="4">
         <v>128</v>
       </c>
@@ -2053,23 +2053,23 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="62"/>
-      <c r="S6" s="47"/>
-      <c r="T6" s="60"/>
-      <c r="U6" s="47"/>
-      <c r="V6" s="47"/>
-      <c r="W6" s="60"/>
-      <c r="X6" s="44"/>
-      <c r="Y6" s="46"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="44"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="46"/>
+      <c r="U6" s="45"/>
+      <c r="V6" s="45"/>
+      <c r="W6" s="46"/>
+      <c r="X6" s="69"/>
+      <c r="Y6" s="71"/>
       <c r="Z6" s="22"/>
       <c r="AA6" s="22"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B7" s="66"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="59" t="s">
+      <c r="B7" s="60"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="50" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="5">
@@ -2109,30 +2109,30 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P7" s="59">
+      <c r="P7" s="50">
         <f>SUM(N7:N8)</f>
         <v>100</v>
       </c>
-      <c r="Q7" s="59">
+      <c r="Q7" s="50">
         <f>SUM(O7:O8)</f>
         <v>20</v>
       </c>
-      <c r="R7" s="63">
+      <c r="R7" s="47">
         <f>SUM(M7:M8)</f>
         <v>62.625</v>
       </c>
-      <c r="S7" s="47"/>
-      <c r="T7" s="60"/>
-      <c r="U7" s="47"/>
-      <c r="V7" s="47"/>
-      <c r="W7" s="60"/>
-      <c r="X7" s="44"/>
-      <c r="Y7" s="46"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="46"/>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="69"/>
+      <c r="Y7" s="71"/>
     </row>
     <row r="8" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B8" s="66"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="59"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="5">
         <v>20</v>
       </c>
@@ -2170,21 +2170,21 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="P8" s="59"/>
-      <c r="Q8" s="59"/>
-      <c r="R8" s="64"/>
-      <c r="S8" s="47"/>
-      <c r="T8" s="60"/>
-      <c r="U8" s="47"/>
-      <c r="V8" s="47"/>
-      <c r="W8" s="60"/>
-      <c r="X8" s="44"/>
-      <c r="Y8" s="46"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="46"/>
+      <c r="U8" s="45"/>
+      <c r="V8" s="45"/>
+      <c r="W8" s="46"/>
+      <c r="X8" s="69"/>
+      <c r="Y8" s="71"/>
     </row>
     <row r="9" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B9" s="66"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47" t="s">
+      <c r="B9" s="60"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="2">
@@ -2224,30 +2224,30 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P9" s="47">
+      <c r="P9" s="45">
         <f>SUM(N9:N10)</f>
         <v>60</v>
       </c>
-      <c r="Q9" s="47">
+      <c r="Q9" s="45">
         <f>SUM(O9:O10)</f>
         <v>20</v>
       </c>
-      <c r="R9" s="61">
+      <c r="R9" s="43">
         <f>SUM(M9:M10)</f>
         <v>32.625</v>
       </c>
-      <c r="S9" s="47"/>
-      <c r="T9" s="60"/>
-      <c r="U9" s="47"/>
-      <c r="V9" s="47"/>
-      <c r="W9" s="60"/>
-      <c r="X9" s="44"/>
-      <c r="Y9" s="46"/>
+      <c r="S9" s="45"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="45"/>
+      <c r="V9" s="45"/>
+      <c r="W9" s="46"/>
+      <c r="X9" s="69"/>
+      <c r="Y9" s="71"/>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B10" s="66"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
       <c r="E10" s="2">
         <v>4</v>
       </c>
@@ -2285,21 +2285,21 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="P10" s="47"/>
-      <c r="Q10" s="47"/>
-      <c r="R10" s="62"/>
-      <c r="S10" s="47"/>
-      <c r="T10" s="60"/>
-      <c r="U10" s="47"/>
-      <c r="V10" s="47"/>
-      <c r="W10" s="60"/>
-      <c r="X10" s="44"/>
-      <c r="Y10" s="46"/>
+      <c r="P10" s="45"/>
+      <c r="Q10" s="45"/>
+      <c r="R10" s="44"/>
+      <c r="S10" s="45"/>
+      <c r="T10" s="46"/>
+      <c r="U10" s="45"/>
+      <c r="V10" s="45"/>
+      <c r="W10" s="46"/>
+      <c r="X10" s="69"/>
+      <c r="Y10" s="71"/>
     </row>
     <row r="11" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B11" s="66"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="59" t="s">
+      <c r="B11" s="60"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="50" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="5">
@@ -2339,30 +2339,30 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P11" s="59">
+      <c r="P11" s="50">
         <f>SUM(N11:N12)</f>
         <v>30</v>
       </c>
-      <c r="Q11" s="59">
+      <c r="Q11" s="50">
         <f>SUM(O11:O12)</f>
         <v>10</v>
       </c>
-      <c r="R11" s="63">
+      <c r="R11" s="47">
         <f>SUM(M11:M12)</f>
         <v>16.3125</v>
       </c>
-      <c r="S11" s="47"/>
-      <c r="T11" s="60"/>
-      <c r="U11" s="47"/>
-      <c r="V11" s="47"/>
-      <c r="W11" s="60"/>
-      <c r="X11" s="44"/>
-      <c r="Y11" s="46"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="46"/>
+      <c r="U11" s="45"/>
+      <c r="V11" s="45"/>
+      <c r="W11" s="46"/>
+      <c r="X11" s="69"/>
+      <c r="Y11" s="71"/>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B12" s="66"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="59"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="50"/>
       <c r="E12" s="5">
         <v>2</v>
       </c>
@@ -2400,20 +2400,20 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="59"/>
-      <c r="R12" s="64"/>
-      <c r="S12" s="47"/>
-      <c r="T12" s="60"/>
-      <c r="U12" s="47"/>
-      <c r="V12" s="47"/>
-      <c r="W12" s="60"/>
-      <c r="X12" s="44"/>
-      <c r="Y12" s="46"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="46"/>
+      <c r="U12" s="45"/>
+      <c r="V12" s="45"/>
+      <c r="W12" s="46"/>
+      <c r="X12" s="69"/>
+      <c r="Y12" s="71"/>
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B13" s="66"/>
-      <c r="C13" s="47"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="6" t="s">
         <v>5</v>
       </c>
@@ -2466,17 +2466,17 @@
         <f>M13</f>
         <v>105.60000000000001</v>
       </c>
-      <c r="S13" s="47"/>
-      <c r="T13" s="60"/>
-      <c r="U13" s="47"/>
-      <c r="V13" s="47"/>
-      <c r="W13" s="60"/>
-      <c r="X13" s="44"/>
-      <c r="Y13" s="46"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="46"/>
+      <c r="U13" s="45"/>
+      <c r="V13" s="45"/>
+      <c r="W13" s="46"/>
+      <c r="X13" s="69"/>
+      <c r="Y13" s="71"/>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B14" s="66"/>
-      <c r="C14" s="47"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="8" t="s">
         <v>6</v>
       </c>
@@ -2529,17 +2529,17 @@
         <f>M14</f>
         <v>88</v>
       </c>
-      <c r="S14" s="47"/>
-      <c r="T14" s="60"/>
-      <c r="U14" s="47"/>
-      <c r="V14" s="47"/>
-      <c r="W14" s="60"/>
-      <c r="X14" s="44"/>
-      <c r="Y14" s="46"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="46"/>
+      <c r="U14" s="45"/>
+      <c r="V14" s="45"/>
+      <c r="W14" s="46"/>
+      <c r="X14" s="69"/>
+      <c r="Y14" s="71"/>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B15" s="66"/>
-      <c r="C15" s="47"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="6" t="s">
         <v>38</v>
       </c>
@@ -2592,20 +2592,20 @@
         <f>M15</f>
         <v>375</v>
       </c>
-      <c r="S15" s="47"/>
-      <c r="T15" s="60"/>
-      <c r="U15" s="47"/>
-      <c r="V15" s="47"/>
-      <c r="W15" s="60"/>
-      <c r="X15" s="44"/>
-      <c r="Y15" s="46"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="46"/>
+      <c r="U15" s="45"/>
+      <c r="V15" s="45"/>
+      <c r="W15" s="46"/>
+      <c r="X15" s="69"/>
+      <c r="Y15" s="71"/>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B16" s="66"/>
-      <c r="C16" s="53" t="s">
+      <c r="B16" s="60"/>
+      <c r="C16" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="59" t="s">
+      <c r="D16" s="50" t="s">
         <v>30</v>
       </c>
       <c r="E16" s="5">
@@ -2646,39 +2646,39 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P16" s="59">
+      <c r="P16" s="50">
         <f>SUM(N16:N17)</f>
         <v>240</v>
       </c>
-      <c r="Q16" s="59">
+      <c r="Q16" s="50">
         <f>SUM(O16:O17)</f>
         <v>80</v>
       </c>
-      <c r="R16" s="63">
+      <c r="R16" s="47">
         <f>SUM(M16:M17)</f>
         <v>130.5</v>
       </c>
-      <c r="S16" s="47">
+      <c r="S16" s="45">
         <f>SUM(P16:P21)</f>
         <v>410</v>
       </c>
-      <c r="T16" s="60">
+      <c r="T16" s="46">
         <f>S16/$C$44</f>
         <v>8.5416666666666661</v>
       </c>
-      <c r="U16" s="47">
+      <c r="U16" s="45">
         <f>SUM(M16:M21)*C34</f>
         <v>808.3125</v>
       </c>
-      <c r="V16" s="47"/>
-      <c r="W16" s="60"/>
-      <c r="X16" s="44"/>
-      <c r="Y16" s="46"/>
+      <c r="V16" s="45"/>
+      <c r="W16" s="46"/>
+      <c r="X16" s="69"/>
+      <c r="Y16" s="71"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B17" s="66"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="59"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="50"/>
       <c r="E17" s="5">
         <v>10</v>
       </c>
@@ -2717,21 +2717,21 @@
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="P17" s="59"/>
-      <c r="Q17" s="59"/>
-      <c r="R17" s="64"/>
-      <c r="S17" s="47"/>
-      <c r="T17" s="60"/>
-      <c r="U17" s="47"/>
-      <c r="V17" s="47"/>
-      <c r="W17" s="60"/>
-      <c r="X17" s="44"/>
-      <c r="Y17" s="46"/>
+      <c r="P17" s="50"/>
+      <c r="Q17" s="50"/>
+      <c r="R17" s="48"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="46"/>
+      <c r="U17" s="45"/>
+      <c r="V17" s="45"/>
+      <c r="W17" s="46"/>
+      <c r="X17" s="69"/>
+      <c r="Y17" s="71"/>
     </row>
     <row r="18" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="66"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="47" t="s">
+      <c r="B18" s="60"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="45" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="2">
@@ -2772,30 +2772,30 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P18" s="48">
+      <c r="P18" s="61">
         <f>SUM(N18:N19)</f>
         <v>60</v>
       </c>
-      <c r="Q18" s="48">
+      <c r="Q18" s="61">
         <f>SUM(O18:O19)</f>
         <v>20</v>
       </c>
-      <c r="R18" s="67">
+      <c r="R18" s="62">
         <f>SUM(M18:M19)</f>
         <v>32.625</v>
       </c>
-      <c r="S18" s="47"/>
-      <c r="T18" s="60"/>
-      <c r="U18" s="47"/>
-      <c r="V18" s="47"/>
-      <c r="W18" s="60"/>
-      <c r="X18" s="44"/>
-      <c r="Y18" s="46"/>
+      <c r="S18" s="45"/>
+      <c r="T18" s="46"/>
+      <c r="U18" s="45"/>
+      <c r="V18" s="45"/>
+      <c r="W18" s="46"/>
+      <c r="X18" s="69"/>
+      <c r="Y18" s="71"/>
     </row>
     <row r="19" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="66"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="47"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="45"/>
       <c r="E19" s="2">
         <v>2</v>
       </c>
@@ -2834,21 +2834,21 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="48"/>
-      <c r="R19" s="68"/>
-      <c r="S19" s="47"/>
-      <c r="T19" s="60"/>
-      <c r="U19" s="47"/>
-      <c r="V19" s="47"/>
-      <c r="W19" s="60"/>
-      <c r="X19" s="44"/>
-      <c r="Y19" s="46"/>
+      <c r="P19" s="61"/>
+      <c r="Q19" s="61"/>
+      <c r="R19" s="63"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="46"/>
+      <c r="U19" s="45"/>
+      <c r="V19" s="45"/>
+      <c r="W19" s="46"/>
+      <c r="X19" s="69"/>
+      <c r="Y19" s="71"/>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B20" s="66"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="59" t="s">
+      <c r="B20" s="60"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="50" t="s">
         <v>32</v>
       </c>
       <c r="E20" s="5">
@@ -2888,30 +2888,30 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P20" s="59">
+      <c r="P20" s="50">
         <f>SUM(N20:N21)</f>
         <v>110</v>
       </c>
-      <c r="Q20" s="59">
+      <c r="Q20" s="50">
         <f>SUM(O20:O21)</f>
         <v>10</v>
       </c>
-      <c r="R20" s="63">
+      <c r="R20" s="47">
         <f>SUM(M20:M21)</f>
         <v>106.3125</v>
       </c>
-      <c r="S20" s="47"/>
-      <c r="T20" s="60"/>
-      <c r="U20" s="47"/>
-      <c r="V20" s="47"/>
-      <c r="W20" s="60"/>
-      <c r="X20" s="44"/>
-      <c r="Y20" s="46"/>
+      <c r="S20" s="45"/>
+      <c r="T20" s="46"/>
+      <c r="U20" s="45"/>
+      <c r="V20" s="45"/>
+      <c r="W20" s="46"/>
+      <c r="X20" s="69"/>
+      <c r="Y20" s="71"/>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B21" s="66"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="59"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="50"/>
       <c r="E21" s="5">
         <v>2</v>
       </c>
@@ -2949,23 +2949,23 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="59"/>
-      <c r="R21" s="64"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="60"/>
-      <c r="U21" s="47"/>
-      <c r="V21" s="47"/>
-      <c r="W21" s="60"/>
-      <c r="X21" s="44"/>
-      <c r="Y21" s="46"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="45"/>
+      <c r="T21" s="46"/>
+      <c r="U21" s="45"/>
+      <c r="V21" s="45"/>
+      <c r="W21" s="46"/>
+      <c r="X21" s="69"/>
+      <c r="Y21" s="71"/>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B22" s="66"/>
-      <c r="C22" s="47">
+      <c r="B22" s="60"/>
+      <c r="C22" s="45">
         <v>5</v>
       </c>
-      <c r="D22" s="48" t="s">
+      <c r="D22" s="61" t="s">
         <v>39</v>
       </c>
       <c r="E22" s="7">
@@ -2977,7 +2977,7 @@
       <c r="G22" s="2">
         <v>2</v>
       </c>
-      <c r="H22" s="69" t="s">
+      <c r="H22" s="57" t="s">
         <v>9</v>
       </c>
       <c r="I22" s="3">
@@ -3005,39 +3005,39 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P22" s="47">
+      <c r="P22" s="45">
         <f>SUM(N22:N23)</f>
         <v>150</v>
       </c>
-      <c r="Q22" s="47">
+      <c r="Q22" s="45">
         <f>SUM(O22:O23)</f>
         <v>50</v>
       </c>
-      <c r="R22" s="61">
+      <c r="R22" s="43">
         <f>SUM(M22:M23)</f>
         <v>81.5625</v>
       </c>
-      <c r="S22" s="47">
+      <c r="S22" s="45">
         <f>SUM(P22:P24)</f>
         <v>162</v>
       </c>
-      <c r="T22" s="60">
+      <c r="T22" s="46">
         <f>S22/$C$44</f>
         <v>3.375</v>
       </c>
-      <c r="U22" s="47">
+      <c r="U22" s="45">
         <f>SUM(M22:M24)</f>
         <v>187.16250000000002</v>
       </c>
-      <c r="V22" s="47"/>
-      <c r="W22" s="60"/>
-      <c r="X22" s="44"/>
-      <c r="Y22" s="46"/>
+      <c r="V22" s="45"/>
+      <c r="W22" s="46"/>
+      <c r="X22" s="69"/>
+      <c r="Y22" s="71"/>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B23" s="66"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="48"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="61"/>
       <c r="E23" s="7">
         <v>50</v>
       </c>
@@ -3047,7 +3047,7 @@
       <c r="G23" s="2">
         <v>1</v>
       </c>
-      <c r="H23" s="69"/>
+      <c r="H23" s="57"/>
       <c r="I23" s="4">
         <v>128</v>
       </c>
@@ -3073,20 +3073,20 @@
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="P23" s="47"/>
-      <c r="Q23" s="47"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="47"/>
-      <c r="T23" s="60"/>
-      <c r="U23" s="47"/>
-      <c r="V23" s="47"/>
-      <c r="W23" s="60"/>
-      <c r="X23" s="44"/>
-      <c r="Y23" s="46"/>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="45"/>
+      <c r="R23" s="44"/>
+      <c r="S23" s="45"/>
+      <c r="T23" s="46"/>
+      <c r="U23" s="45"/>
+      <c r="V23" s="45"/>
+      <c r="W23" s="46"/>
+      <c r="X23" s="69"/>
+      <c r="Y23" s="71"/>
     </row>
     <row r="24" spans="2:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="66"/>
-      <c r="C24" s="47"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="45"/>
       <c r="D24" s="8" t="s">
         <v>5</v>
       </c>
@@ -3139,22 +3139,22 @@
         <f>M24</f>
         <v>105.60000000000001</v>
       </c>
-      <c r="S24" s="47"/>
-      <c r="T24" s="60"/>
-      <c r="U24" s="47"/>
-      <c r="V24" s="47"/>
-      <c r="W24" s="60"/>
-      <c r="X24" s="44"/>
-      <c r="Y24" s="46"/>
+      <c r="S24" s="45"/>
+      <c r="T24" s="46"/>
+      <c r="U24" s="45"/>
+      <c r="V24" s="45"/>
+      <c r="W24" s="46"/>
+      <c r="X24" s="69"/>
+      <c r="Y24" s="71"/>
     </row>
     <row r="25" spans="2:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="53" t="s">
+      <c r="C25" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="50" t="s">
+      <c r="D25" s="66" t="s">
         <v>49</v>
       </c>
       <c r="E25" s="7">
@@ -3166,7 +3166,7 @@
       <c r="G25" s="7">
         <v>4</v>
       </c>
-      <c r="H25" s="57" t="s">
+      <c r="H25" s="67" t="s">
         <v>54</v>
       </c>
       <c r="I25" s="12">
@@ -3202,37 +3202,37 @@
         <f>SUM(O25:O26)</f>
         <v>50</v>
       </c>
-      <c r="R25" s="61">
+      <c r="R25" s="43">
         <f>SUM(M25:M26)</f>
         <v>156.5625</v>
       </c>
-      <c r="S25" s="50">
+      <c r="S25" s="66">
         <f>SUM(P25)</f>
         <v>250</v>
       </c>
-      <c r="T25" s="51">
+      <c r="T25" s="73">
         <f>S25/$C$44</f>
         <v>5.208333333333333</v>
       </c>
-      <c r="U25" s="50">
+      <c r="U25" s="66">
         <f>SUM(M25:M26)</f>
         <v>156.5625</v>
       </c>
-      <c r="V25" s="52">
+      <c r="V25" s="74">
         <f>U25*C35+U27+U28</f>
         <v>826.25</v>
       </c>
-      <c r="W25" s="49">
+      <c r="W25" s="72">
         <f>T25+T27*C35+T28</f>
         <v>23.958333333333332</v>
       </c>
-      <c r="X25" s="44"/>
-      <c r="Y25" s="46"/>
+      <c r="X25" s="69"/>
+      <c r="Y25" s="71"/>
     </row>
     <row r="26" spans="2:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="54"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="50"/>
+      <c r="B26" s="64"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="66"/>
       <c r="E26" s="7">
         <v>50</v>
       </c>
@@ -3242,7 +3242,7 @@
       <c r="G26" s="7">
         <v>1</v>
       </c>
-      <c r="H26" s="57"/>
+      <c r="H26" s="67"/>
       <c r="I26" s="13">
         <v>128</v>
       </c>
@@ -3270,17 +3270,17 @@
       </c>
       <c r="P26" s="56"/>
       <c r="Q26" s="56"/>
-      <c r="R26" s="62"/>
-      <c r="S26" s="50"/>
-      <c r="T26" s="51"/>
-      <c r="U26" s="50"/>
-      <c r="V26" s="52"/>
-      <c r="W26" s="49"/>
-      <c r="X26" s="44"/>
-      <c r="Y26" s="46"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="66"/>
+      <c r="T26" s="73"/>
+      <c r="U26" s="66"/>
+      <c r="V26" s="74"/>
+      <c r="W26" s="72"/>
+      <c r="X26" s="69"/>
+      <c r="Y26" s="71"/>
     </row>
     <row r="27" spans="2:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="54"/>
+      <c r="B27" s="64"/>
       <c r="C27" s="8">
         <v>4</v>
       </c>
@@ -3348,17 +3348,17 @@
         <f>SUM(M27)</f>
         <v>275</v>
       </c>
-      <c r="V27" s="52"/>
-      <c r="W27" s="49"/>
-      <c r="X27" s="44"/>
-      <c r="Y27" s="46"/>
+      <c r="V27" s="74"/>
+      <c r="W27" s="72"/>
+      <c r="X27" s="69"/>
+      <c r="Y27" s="71"/>
     </row>
     <row r="28" spans="2:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="54"/>
-      <c r="C28" s="47">
+      <c r="B28" s="64"/>
+      <c r="C28" s="45">
         <v>5</v>
       </c>
-      <c r="D28" s="50" t="s">
+      <c r="D28" s="66" t="s">
         <v>52</v>
       </c>
       <c r="E28" s="7">
@@ -3370,7 +3370,7 @@
       <c r="G28" s="7">
         <v>2</v>
       </c>
-      <c r="H28" s="55" t="s">
+      <c r="H28" s="65" t="s">
         <v>50</v>
       </c>
       <c r="I28" s="12">
@@ -3406,31 +3406,31 @@
         <f>SUM(O28:O29)</f>
         <v>50</v>
       </c>
-      <c r="R28" s="61">
+      <c r="R28" s="43">
         <f>SUM(M28:M29)</f>
         <v>81.5625</v>
       </c>
-      <c r="S28" s="50">
+      <c r="S28" s="66">
         <f>SUM(P28)</f>
         <v>150</v>
       </c>
-      <c r="T28" s="51">
+      <c r="T28" s="73">
         <f>S28/$C$44</f>
         <v>3.125</v>
       </c>
-      <c r="U28" s="50">
+      <c r="U28" s="66">
         <f>SUM(M28:M29)</f>
         <v>81.5625</v>
       </c>
-      <c r="V28" s="52"/>
-      <c r="W28" s="49"/>
-      <c r="X28" s="44"/>
-      <c r="Y28" s="46"/>
+      <c r="V28" s="74"/>
+      <c r="W28" s="72"/>
+      <c r="X28" s="69"/>
+      <c r="Y28" s="71"/>
     </row>
     <row r="29" spans="2:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="54"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="50"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="66"/>
       <c r="E29" s="7">
         <v>50</v>
       </c>
@@ -3440,7 +3440,7 @@
       <c r="G29" s="7">
         <v>1</v>
       </c>
-      <c r="H29" s="55"/>
+      <c r="H29" s="65"/>
       <c r="I29" s="13">
         <v>128</v>
       </c>
@@ -3468,14 +3468,14 @@
       </c>
       <c r="P29" s="56"/>
       <c r="Q29" s="56"/>
-      <c r="R29" s="62"/>
-      <c r="S29" s="50"/>
-      <c r="T29" s="51"/>
-      <c r="U29" s="50"/>
-      <c r="V29" s="52"/>
-      <c r="W29" s="49"/>
-      <c r="X29" s="44"/>
-      <c r="Y29" s="46"/>
+      <c r="R29" s="44"/>
+      <c r="S29" s="66"/>
+      <c r="T29" s="73"/>
+      <c r="U29" s="66"/>
+      <c r="V29" s="74"/>
+      <c r="W29" s="72"/>
+      <c r="X29" s="69"/>
+      <c r="Y29" s="71"/>
     </row>
     <row r="30" spans="2:25" ht="53.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B30" s="41" t="s">
@@ -3545,8 +3545,8 @@
         <f>R30</f>
         <v>590.76923076923083</v>
       </c>
-      <c r="X30" s="44"/>
-      <c r="Y30" s="46"/>
+      <c r="X30" s="69"/>
+      <c r="Y30" s="71"/>
     </row>
     <row r="31" spans="2:25" x14ac:dyDescent="0.25">
       <c r="O31" s="1">
@@ -3839,12 +3839,12 @@
       <c r="H42" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I42" s="65">
+      <c r="I42" s="58">
         <f>SUM(F32:F38)</f>
         <v>2134790.9570833333</v>
       </c>
-      <c r="J42" s="65"/>
-      <c r="K42" s="65"/>
+      <c r="J42" s="58"/>
+      <c r="K42" s="58"/>
       <c r="O42" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -3884,30 +3884,46 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="T5:T15"/>
-    <mergeCell ref="U5:U15"/>
-    <mergeCell ref="R9:R10"/>
-    <mergeCell ref="R11:R12"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="R25:R26"/>
-    <mergeCell ref="P28:P29"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="X5:X30"/>
+    <mergeCell ref="Y5:Y30"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="C5:C15"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="W25:W29"/>
+    <mergeCell ref="S28:S29"/>
+    <mergeCell ref="T28:T29"/>
+    <mergeCell ref="U28:U29"/>
+    <mergeCell ref="S25:S26"/>
+    <mergeCell ref="T25:T26"/>
+    <mergeCell ref="U25:U26"/>
+    <mergeCell ref="V25:V29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B25:B29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="Q28:Q29"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="Q25:Q26"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="W5:W24"/>
+    <mergeCell ref="U16:U21"/>
+    <mergeCell ref="T16:T21"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="V5:V24"/>
+    <mergeCell ref="T22:T24"/>
+    <mergeCell ref="U22:U24"/>
+    <mergeCell ref="S5:S15"/>
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="S16:S21"/>
+    <mergeCell ref="R7:R8"/>
     <mergeCell ref="I42:K42"/>
     <mergeCell ref="C16:C21"/>
     <mergeCell ref="B5:B24"/>
@@ -3924,46 +3940,30 @@
     <mergeCell ref="R16:R17"/>
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="R20:R21"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="P20:P21"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="W5:W24"/>
-    <mergeCell ref="U16:U21"/>
-    <mergeCell ref="T16:T21"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="V5:V24"/>
-    <mergeCell ref="T22:T24"/>
-    <mergeCell ref="U22:U24"/>
-    <mergeCell ref="S5:S15"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="S16:S21"/>
-    <mergeCell ref="R7:R8"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="Q28:Q29"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="Q25:Q26"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="X5:X30"/>
-    <mergeCell ref="Y5:Y30"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="C5:C15"/>
-    <mergeCell ref="Q9:Q10"/>
-    <mergeCell ref="W25:W29"/>
-    <mergeCell ref="S28:S29"/>
-    <mergeCell ref="T28:T29"/>
-    <mergeCell ref="U28:U29"/>
-    <mergeCell ref="S25:S26"/>
-    <mergeCell ref="T25:T26"/>
-    <mergeCell ref="U25:U26"/>
-    <mergeCell ref="V25:V29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="R25:R26"/>
+    <mergeCell ref="P28:P29"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="R5:R6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="T5:T15"/>
+    <mergeCell ref="U5:U15"/>
+    <mergeCell ref="R9:R10"/>
+    <mergeCell ref="R11:R12"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="Q11:Q12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3980,7 +3980,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="124" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4671,10 +4671,10 @@
         <v>168</v>
       </c>
       <c r="I35" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J35" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="K35" t="s">
         <v>104</v>

</xml_diff>